<commit_message>
Working after initial upload changed the directy name.
</commit_message>
<xml_diff>
--- a/CreateManifest.xlsx
+++ b/CreateManifest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gebirecki\protractorworkspace\Protractor6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gebirecki\protractorworkspace\ProtractorAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,14 +14,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="Date">Sheet1!$K$4</definedName>
-    <definedName name="Notes">Sheet1!$K$6</definedName>
-    <definedName name="PO">Sheet1!$K$8</definedName>
-    <definedName name="SO">Sheet1!$K$7</definedName>
-    <definedName name="Time">Sheet1!$K$5</definedName>
-    <definedName name="Truck">Sheet1!$K$9</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,14 +24,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="59">
+  <si>
+    <t>Shipping Manifest Automation Test</t>
+  </si>
   <si>
     <t>http://webservicedev.winwholesale.com/shipping-manifest-manager-release/#/list</t>
   </si>
   <si>
-    <t>This URL is company 615</t>
-  </si>
-  <si>
     <t>Test Name</t>
   </si>
   <si>
@@ -76,57 +68,57 @@
     <t>Date</t>
   </si>
   <si>
+    <t>01/30/2019</t>
+  </si>
+  <si>
+    <t>verifyInput</t>
+  </si>
+  <si>
+    <t>input#newManifestDeliveryDate</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Drop it off</t>
+  </si>
+  <si>
+    <t>clearSendKeys</t>
+  </si>
+  <si>
+    <t>input#newManifestStartTime</t>
+  </si>
+  <si>
+    <t>12:00 PM</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>406087-01</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>059127</t>
+  </si>
+  <si>
+    <t>Truck</t>
+  </si>
+  <si>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>selectDropDown</t>
+  </si>
+  <si>
+    <t>#truck &gt; option</t>
+  </si>
+  <si>
     <t>sendKeys</t>
   </si>
   <si>
-    <t>input#newManifestDeliveryDate</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>12:00 PM</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Drop it off</t>
-  </si>
-  <si>
-    <t>clearSendKeys</t>
-  </si>
-  <si>
-    <t>input#newManifestStartTime</t>
-  </si>
-  <si>
-    <t>SO</t>
-  </si>
-  <si>
-    <t>406087-01</t>
-  </si>
-  <si>
-    <t>PO</t>
-  </si>
-  <si>
-    <t>059127</t>
-  </si>
-  <si>
-    <t>#truck[name="truck"]</t>
-  </si>
-  <si>
-    <t>Truck</t>
-  </si>
-  <si>
-    <t>Nissan</t>
-  </si>
-  <si>
-    <t>selectDropDown</t>
-  </si>
-  <si>
-    <t>#truck &gt; option</t>
-  </si>
-  <si>
     <t>textarea#notes</t>
   </si>
   <si>
@@ -148,6 +140,9 @@
     <t>#collapseStop0 &gt; div &gt; div &gt; div &gt; div &gt; p-messages &gt; div &gt; ul &gt; li &gt; span.ui-messages-summary</t>
   </si>
   <si>
+    <t>Order 406087-01 successfully added to manifest</t>
+  </si>
+  <si>
     <t>Create Manifest - Add PO</t>
   </si>
   <si>
@@ -157,15 +152,6 @@
     <t>#newManifestModal &gt; new-manifest &gt; div.modal-dialog &gt; div &gt; div &gt; div.add-po-content.container.footerMargin &gt; div &gt; div.row &gt; form &gt; div.form-group.col-lg-8.col-md-8.col-sm-8.col-xs-12 &gt; input</t>
   </si>
   <si>
-    <t>sendCmdKeys</t>
-  </si>
-  <si>
-    <t>input[placeholder="Order/Vendor Number, Vendor Name, Address"]</t>
-  </si>
-  <si>
-    <t>protractor.Key.PAGE_DOWN</t>
-  </si>
-  <si>
     <t>#newManifestModal &gt; new-manifest &gt; div.modal-dialog &gt; div &gt; div &gt; div.add-po-content.container.footerMargin &gt; div &gt; div.po-content &gt; p-datatable &gt; div &gt; div.ui-datatable-tablewrapper &gt; table &gt; tbody &gt; tr &gt; td:nth-child(1)</t>
   </si>
   <si>
@@ -178,6 +164,9 @@
     <t>#collapseStop1 &gt; div &gt; div &gt; div &gt; div &gt; p-messages &gt; div &gt; ul &gt; li &gt; span.ui-messages-summary</t>
   </si>
   <si>
+    <t>Order 059127 successfully added to manifest</t>
+  </si>
+  <si>
     <t>#newManifestModal &gt; new-manifest &gt; div.action-buttons &gt; div &gt; div &gt; div.right &gt; button &gt; span</t>
   </si>
   <si>
@@ -205,19 +194,13 @@
     <t>#deleteManifestModal &gt; div &gt; div &gt; div &gt; div &gt; div:nth-child(4) &gt; button.btn.win-confirmation-btn-blue.background-blue</t>
   </si>
   <si>
-    <t>Shipping Manifest Automation Test</t>
-  </si>
-  <si>
-    <t>Order 406087-01 successfully added to manifest</t>
-  </si>
-  <si>
-    <t>Order 059127 successfully added to manifest</t>
-  </si>
-  <si>
-    <t>verifyInput</t>
-  </si>
-  <si>
-    <t>01/30/2019</t>
+    <t>verifySelect</t>
+  </si>
+  <si>
+    <t>sendPGDN</t>
+  </si>
+  <si>
+    <t>select#truck:nth-child(1)</t>
   </si>
 </sst>
 </file>
@@ -265,7 +248,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -547,33 +530,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="82" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="72.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -613,11 +591,14 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
+      <c r="F4">
+        <v>3000</v>
+      </c>
       <c r="J4" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>61</v>
+      <c r="K4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -625,23 +606,22 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="str">
-        <f>Date</f>
-        <v>01/30/2019</v>
-      </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -649,23 +629,22 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="str">
-        <f>Date</f>
-        <v>01/30/2019</v>
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -673,23 +652,22 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" t="str">
-        <f>Time</f>
-        <v>12:00 PM</v>
-      </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -697,23 +675,22 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="str">
-        <f>Time</f>
-        <v>12:00 PM</v>
-      </c>
       <c r="J8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -721,19 +698,19 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
         <v>27</v>
       </c>
-      <c r="K9" t="s">
-        <v>28</v>
+      <c r="F9">
+        <v>3000</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -741,17 +718,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" t="str">
-        <f>Truck</f>
-        <v>Nissan</v>
+        <v>58</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -759,7 +735,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -767,9 +743,8 @@
       <c r="D11" t="s">
         <v>31</v>
       </c>
-      <c r="E11" t="str">
-        <f>Notes</f>
-        <v>Drop it off</v>
+      <c r="E11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -777,7 +752,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -785,9 +760,8 @@
       <c r="D12" t="s">
         <v>31</v>
       </c>
-      <c r="E12" t="str">
-        <f>Notes</f>
-        <v>Drop it off</v>
+      <c r="E12" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -803,9 +777,8 @@
       <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="E13" t="str">
-        <f>SO</f>
-        <v>406087-01</v>
+      <c r="E13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -821,9 +794,8 @@
       <c r="D14" t="s">
         <v>36</v>
       </c>
-      <c r="E14" t="str">
-        <f>SO</f>
-        <v>406087-01</v>
+      <c r="E14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -840,12 +812,12 @@
         <v>37</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -854,7 +826,7 @@
         <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F16">
         <v>3000</v>
@@ -862,28 +834,27 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" t="str">
-        <f>PO</f>
-        <v>059127</v>
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -891,13 +862,10 @@
       <c r="D18" t="s">
         <v>42</v>
       </c>
-      <c r="E18" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
@@ -906,26 +874,32 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20">
+        <v>2000</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
         <v>35</v>
@@ -934,22 +908,18 @@
         <v>11</v>
       </c>
       <c r="D21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" t="s">
         <v>46</v>
-      </c>
-      <c r="E21" t="str">
-        <f>PO</f>
-        <v>059127</v>
-      </c>
-      <c r="F21">
-        <v>2000</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -957,8 +927,8 @@
       <c r="D22" t="s">
         <v>47</v>
       </c>
-      <c r="E22" t="s">
-        <v>59</v>
+      <c r="F22">
+        <v>2000</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -966,35 +936,35 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23">
-        <v>2000</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="F24">
+        <v>2000</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -1011,7 +981,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -1022,13 +992,10 @@
       <c r="D26" t="s">
         <v>53</v>
       </c>
-      <c r="F26">
-        <v>2000</v>
-      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -1042,7 +1009,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -1053,36 +1020,22 @@
       <c r="D28" t="s">
         <v>55</v>
       </c>
+      <c r="F28">
+        <v>1000</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
         <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" t="s">
         <v>49</v>
-      </c>
-      <c r="C30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1090,6 +1043,5 @@
     <hyperlink ref="A2" r:id="rId1" location="/list"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>